<commit_message>
add zone import new format
</commit_message>
<xml_diff>
--- a/public/sample/zone_bulkimport.xlsx
+++ b/public/sample/zone_bulkimport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\easemylr-pro\public\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F38BA5-8B07-423C-88FA-C6269C25CA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEB40EF-67BB-4E38-A508-0CF09056FECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85FD23C3-00A6-4522-A24E-8D9CC9FD1E86}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Primary Zone</t>
   </si>
@@ -47,13 +47,28 @@
   </si>
   <si>
     <t>Postal Code</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>SAS Nagar</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>Ludhiana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +79,12 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -94,18 +115,18 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,43 +441,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25DE1D91-956C-4240-920B-E8BD4D47F8B9}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>282001</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>204102</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="119" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>